<commit_message>
Output interface working for input_data example in main class
</commit_message>
<xml_diff>
--- a/data/receipts/excel_receipts/cube_compression_receipt.xlsx
+++ b/data/receipts/excel_receipts/cube_compression_receipt.xlsx
@@ -20,10 +20,10 @@
     <t/>
   </si>
   <si>
-    <t>Rezultatele încercării:</t>
-  </si>
-  <si>
-    <t>Indicativ serie SAMPLE_001</t>
+    <t>Rezultatele Ã®ncercÄƒrii:</t>
+  </si>
+  <si>
+    <t>Indicativ serie 13</t>
   </si>
   <si>
     <t>1</t>
@@ -38,16 +38,16 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Data confecționării</t>
-  </si>
-  <si>
-    <t>2024-01-15</t>
-  </si>
-  <si>
-    <t>Data încercării</t>
-  </si>
-  <si>
-    <t>2024-01-22</t>
+    <t>Data confecÈ›ionÄƒrii</t>
+  </si>
+  <si>
+    <t>04.06.2025</t>
+  </si>
+  <si>
+    <t>Data Ã®ncercÄƒrii</t>
+  </si>
+  <si>
+    <t>08.06.2025</t>
   </si>
   <si>
     <t>Dimensiunile cubului [mm]</t>
@@ -62,19 +62,19 @@
     <t>z [mm]</t>
   </si>
   <si>
-    <t>Suprafața de compresiune [mm²]</t>
+    <t>SuprafaÈ›a de compresiune [mmÂ²]</t>
   </si>
   <si>
     <t>Greutatea cubului [kg]</t>
   </si>
   <si>
-    <t>Densitatea specifică aparentă [kg/m³]</t>
+    <t>Densitatea specificÄƒ aparentÄƒ [kg/mÂ³]</t>
   </si>
   <si>
     <t>Sarcina de rupere la compresiune [N]</t>
   </si>
   <si>
-    <t>Rezistența de rupere la compresiune [N/mm²]</t>
+    <t>RezistenÈ›a de rupere la compresiune [N/mmÂ²]</t>
   </si>
 </sst>
 </file>
@@ -586,13 +586,13 @@
       </c>
       <c r="B10" s="69"/>
       <c r="C10" t="n" s="70">
-        <v>7.85</v>
+        <v>7.649</v>
       </c>
       <c r="D10" t="n" s="71">
-        <v>7.92</v>
+        <v>7.55</v>
       </c>
       <c r="E10" t="n" s="72">
-        <v>7.78</v>
+        <v>7.609</v>
       </c>
       <c r="F10" s="73">
         <f>AVERAGE(C10:E10)</f>
@@ -622,13 +622,13 @@
       </c>
       <c r="B12" s="81"/>
       <c r="C12" t="n" s="82">
-        <v>425500.0</v>
+        <v>701000.0</v>
       </c>
       <c r="D12" t="n" s="83">
-        <v>438200.0</v>
+        <v>681600.0</v>
       </c>
       <c r="E12" t="n" s="84">
-        <v>412800.0</v>
+        <v>716100.0</v>
       </c>
       <c r="F12" s="85">
         <f>AVERAGE(C12:E12)</f>

</xml_diff>